<commit_message>
Atualização dos registros do projeto
Registro:

. Evolução
. Pendências
. Problemas
</commit_message>
<xml_diff>
--- a/Anotações.xlsx
+++ b/Anotações.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows\Documents\Meus  projetos\TCC-PIV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F33C17AE-5DC3-4CD4-B486-6D3008C43BC6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8CFE6A6-6471-4A52-818B-4051AA1FCA3A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" tabRatio="896" xr2:uid="{1A9FFD6D-C9C1-438C-A886-F2779451949A}"/>
   </bookViews>
   <sheets>
     <sheet name="Evolução" sheetId="3" r:id="rId1"/>
-    <sheet name="TELAS" sheetId="19" r:id="rId2"/>
-    <sheet name="dados" sheetId="2" r:id="rId3"/>
-    <sheet name="PI005_A2" sheetId="23" r:id="rId4"/>
-    <sheet name="Servidor" sheetId="26" r:id="rId5"/>
-    <sheet name="Links de referência" sheetId="1" r:id="rId6"/>
+    <sheet name="Problemas" sheetId="27" r:id="rId2"/>
+    <sheet name="TELAS" sheetId="19" r:id="rId3"/>
+    <sheet name="dados" sheetId="2" r:id="rId4"/>
+    <sheet name="PI005_A2" sheetId="23" r:id="rId5"/>
+    <sheet name="Servidor" sheetId="26" r:id="rId6"/>
+    <sheet name="Links de referência" sheetId="1" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="350">
   <si>
     <t>ESP8266 - NODEMCU</t>
   </si>
@@ -653,9 +654,6 @@
     <t>https://randomnerdtutorials.com/esp8266-nodemcu-hc-sr04-ultrasonic-arduino/</t>
   </si>
   <si>
-    <t>HC-SR04</t>
-  </si>
-  <si>
     <r>
       <t>#include</t>
     </r>
@@ -6745,12 +6743,105 @@
   <si>
     <t>ATENÇÃO!!! Avaliar como hospedar as páginas na nuvem (máquina pessoal como servidor ou serviço na nuvem)</t>
   </si>
+  <si>
+    <t>https://portal.vidadesilicio.com.br/hc-sr04-sensor-ultrassonico/</t>
+  </si>
+  <si>
+    <t>https://forum.arduino.cc/t/hc-sr04-and-esp8266-power-problem/1189793</t>
+  </si>
+  <si>
+    <t>5.</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Sucesso na obtenção de dados de temperatura (field 1)</t>
+  </si>
+  <si>
+    <t>. Implementar padrão de escala em:</t>
+  </si>
+  <si>
+    <t>- Horas</t>
+  </si>
+  <si>
+    <t>- Dias</t>
+  </si>
+  <si>
+    <t>- Semanas</t>
+  </si>
+  <si>
+    <t>. Implementar para o nível</t>
+  </si>
+  <si>
+    <t>6.</t>
+  </si>
+  <si>
+    <t>Diversas atualizações no frontend</t>
+  </si>
+  <si>
+    <t>. Implementadas mensagens de orientação nos elementos</t>
+  </si>
+  <si>
+    <t>. Arrendodar para dois digitos a indicação</t>
+  </si>
+  <si>
+    <t>. Ajustar o retorno de status da API, implementando variável de último estado válido</t>
+  </si>
+  <si>
+    <t>. Implementar a escrita individual para os valores do atuomatismo</t>
+  </si>
+  <si>
+    <t>Tela comando</t>
+  </si>
+  <si>
+    <t>Tela dados</t>
+  </si>
+  <si>
+    <t>. Implementar os resultados</t>
+  </si>
+  <si>
+    <t>. Ajustar gráfico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7. </t>
+  </si>
+  <si>
+    <t>Implementação sensores</t>
+  </si>
+  <si>
+    <t>. Sensor de temperatura OK</t>
+  </si>
+  <si>
+    <t>. Sensor de nível funcionou, porém queimou em função do regulador de tensão.</t>
+  </si>
+  <si>
+    <t>Atualização Hardware</t>
+  </si>
+  <si>
+    <t>. Regulador de tensão - após montagem na caixa só dispara 12Vcc nas saídas</t>
+  </si>
+  <si>
+    <t>. protoboards instaladas provisoriamente na caixa e.</t>
+  </si>
+  <si>
+    <t>. Necessário instalar os relés em paralelo com os led (saídas para bomba e aquecedor)</t>
+  </si>
+  <si>
+    <t>`- Implementar a estrutura no tanque</t>
+  </si>
+  <si>
+    <t>`- Fazer diagrama de interligação</t>
+  </si>
+  <si>
+    <t>`- Fazer desenho layout montagem</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="25">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -6916,6 +7007,14 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -7069,7 +7168,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -7214,6 +7313,9 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -7226,8 +7328,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="24" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -7248,6 +7352,110 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>30480</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>350520</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="CaixaDeTexto 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46D1019A-12E5-49CB-8747-D3BFD3CDB2A8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7726680" y="1950720"/>
+          <a:ext cx="5013960" cy="1165860"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100"/>
+            <a:t>Atenção!!!</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100"/>
+            <a:t>O thingspeak grátis permite</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" baseline="0"/>
+            <a:t> apenas uma intervenção a cada 15s, assim todo comando / informação deve ser enviado individualmente.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100"/>
+            <a:t>. Pensar em uma maneira de desabilitar a página neste intervalo de tempo e habilitar apenas após</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" baseline="0"/>
+            <a:t> 15s.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="pt-BR" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -7340,7 +7548,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -8073,10 +8281,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{272C5EE4-895D-4CDE-9CA6-E2FD39887CEB}">
-  <dimension ref="A1:W61"/>
+  <dimension ref="A1:W48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L44" sqref="L44"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -8146,35 +8354,39 @@
         <v>154</v>
       </c>
       <c r="B10" s="50" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="11" spans="1:23">
       <c r="C11" s="52" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="12" spans="1:23">
       <c r="C12" s="50" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23">
+      <c r="A13" s="52" t="s">
+        <v>322</v>
+      </c>
+      <c r="B13" s="52"/>
+      <c r="C13" s="67" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="13" spans="1:23">
-      <c r="A13" s="52"/>
-      <c r="B13" s="52"/>
-      <c r="C13" s="52" t="s">
-        <v>289</v>
-      </c>
-      <c r="D13" s="52"/>
-      <c r="E13" s="52"/>
-      <c r="F13" s="52"/>
-      <c r="G13" s="52"/>
-      <c r="H13" s="52"/>
-      <c r="I13" s="52"/>
-      <c r="J13" s="52"/>
-      <c r="K13" s="52"/>
-      <c r="L13" s="52"/>
-      <c r="M13" s="52"/>
+      <c r="D13" s="67"/>
+      <c r="E13" s="67"/>
+      <c r="F13" s="67"/>
+      <c r="G13" s="67"/>
+      <c r="H13" s="67"/>
+      <c r="I13" s="67"/>
+      <c r="J13" s="67"/>
+      <c r="K13" s="67"/>
+      <c r="L13" s="67"/>
+      <c r="M13" s="68" t="s">
+        <v>322</v>
+      </c>
       <c r="N13" s="52"/>
       <c r="O13" s="52"/>
       <c r="P13" s="52"/>
@@ -8187,21 +8399,25 @@
       <c r="W13" s="52"/>
     </row>
     <row r="14" spans="1:23">
-      <c r="A14" s="52"/>
+      <c r="A14" s="52" t="s">
+        <v>322</v>
+      </c>
       <c r="B14" s="52"/>
-      <c r="C14" s="52" t="s">
-        <v>290</v>
-      </c>
-      <c r="D14" s="52"/>
-      <c r="E14" s="52"/>
-      <c r="F14" s="52"/>
-      <c r="G14" s="52"/>
-      <c r="H14" s="52"/>
-      <c r="I14" s="52"/>
-      <c r="J14" s="52"/>
-      <c r="K14" s="52"/>
-      <c r="L14" s="52"/>
-      <c r="M14" s="52"/>
+      <c r="C14" s="67" t="s">
+        <v>289</v>
+      </c>
+      <c r="D14" s="67"/>
+      <c r="E14" s="67"/>
+      <c r="F14" s="67"/>
+      <c r="G14" s="67"/>
+      <c r="H14" s="67"/>
+      <c r="I14" s="67"/>
+      <c r="J14" s="67"/>
+      <c r="K14" s="67"/>
+      <c r="L14" s="67"/>
+      <c r="M14" s="68" t="s">
+        <v>322</v>
+      </c>
       <c r="N14" s="52"/>
       <c r="O14" s="52"/>
       <c r="P14" s="52"/>
@@ -8239,13 +8455,12 @@
       <c r="W15" s="52"/>
     </row>
     <row r="16" spans="1:23">
-      <c r="A16" s="52"/>
-      <c r="B16" s="52"/>
-      <c r="C16" s="50" t="s">
-        <v>298</v>
-      </c>
-      <c r="D16" s="52"/>
-      <c r="E16" s="52"/>
+      <c r="A16" s="49" t="s">
+        <v>162</v>
+      </c>
+      <c r="B16" s="50" t="s">
+        <v>306</v>
+      </c>
       <c r="F16" s="52"/>
       <c r="G16" s="52"/>
       <c r="H16" s="52"/>
@@ -8267,10 +8482,9 @@
     </row>
     <row r="17" spans="1:23">
       <c r="A17" s="52"/>
-      <c r="B17" s="52"/>
-      <c r="C17" s="52"/>
-      <c r="D17" s="52"/>
-      <c r="E17" s="52"/>
+      <c r="C17" s="52" t="s">
+        <v>314</v>
+      </c>
       <c r="F17" s="52"/>
       <c r="G17" s="52"/>
       <c r="H17" s="52"/>
@@ -8292,12 +8506,9 @@
     </row>
     <row r="18" spans="1:23">
       <c r="A18" s="52"/>
-      <c r="B18" s="52"/>
       <c r="C18" s="52" t="s">
-        <v>297</v>
-      </c>
-      <c r="D18" s="52"/>
-      <c r="E18" s="52"/>
+        <v>312</v>
+      </c>
       <c r="F18" s="52"/>
       <c r="G18" s="52"/>
       <c r="H18" s="52"/>
@@ -8318,12 +8529,9 @@
       <c r="W18" s="52"/>
     </row>
     <row r="19" spans="1:23">
-      <c r="A19" s="52"/>
       <c r="B19" s="52"/>
       <c r="C19" s="52"/>
-      <c r="D19" s="52" t="s">
-        <v>291</v>
-      </c>
+      <c r="D19" s="52"/>
       <c r="E19" s="52"/>
       <c r="F19" s="52"/>
       <c r="G19" s="52"/>
@@ -8339,17 +8547,13 @@
       <c r="Q19" s="52"/>
       <c r="R19" s="52"/>
       <c r="S19" s="52"/>
-      <c r="T19" s="52"/>
-      <c r="U19" s="52"/>
-      <c r="V19" s="52"/>
-      <c r="W19" s="52"/>
     </row>
     <row r="20" spans="1:23">
-      <c r="A20" s="52"/>
-      <c r="B20" s="52"/>
-      <c r="C20" s="52"/>
-      <c r="D20" s="52" t="s">
-        <v>292</v>
+      <c r="A20" s="49" t="s">
+        <v>321</v>
+      </c>
+      <c r="B20" s="50" t="s">
+        <v>323</v>
       </c>
       <c r="E20" s="52"/>
       <c r="F20" s="52"/>
@@ -8366,18 +8570,11 @@
       <c r="Q20" s="52"/>
       <c r="R20" s="52"/>
       <c r="S20" s="52"/>
-      <c r="T20" s="52"/>
-      <c r="U20" s="52"/>
-      <c r="V20" s="52"/>
-      <c r="W20" s="52"/>
     </row>
     <row r="21" spans="1:23">
-      <c r="A21" s="52"/>
       <c r="B21" s="52"/>
       <c r="C21" s="52"/>
-      <c r="D21" s="52" t="s">
-        <v>293</v>
-      </c>
+      <c r="D21" s="52"/>
       <c r="E21" s="52"/>
       <c r="F21" s="52"/>
       <c r="G21" s="52"/>
@@ -8393,18 +8590,577 @@
       <c r="Q21" s="52"/>
       <c r="R21" s="52"/>
       <c r="S21" s="52"/>
-      <c r="T21" s="52"/>
-      <c r="U21" s="52"/>
-      <c r="V21" s="52"/>
-      <c r="W21" s="52"/>
     </row>
     <row r="22" spans="1:23">
-      <c r="A22" s="52"/>
+      <c r="A22" s="49" t="s">
+        <v>329</v>
+      </c>
+      <c r="B22" s="50" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23">
+      <c r="B23" s="50" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23">
+      <c r="B24" s="53" t="s">
+        <v>331</v>
+      </c>
+      <c r="C24" s="53"/>
+      <c r="D24" s="53"/>
+    </row>
+    <row r="25" spans="1:23">
+      <c r="B25" s="53" t="s">
+        <v>332</v>
+      </c>
+      <c r="C25" s="53"/>
+      <c r="D25" s="53"/>
+    </row>
+    <row r="26" spans="1:23">
+      <c r="B26" s="53" t="s">
+        <v>333</v>
+      </c>
+      <c r="C26" s="53"/>
+      <c r="D26" s="53"/>
+    </row>
+    <row r="27" spans="1:23">
+      <c r="B27" s="53" t="s">
+        <v>334</v>
+      </c>
+      <c r="C27" s="53"/>
+      <c r="D27" s="53"/>
+    </row>
+    <row r="28" spans="1:23">
+      <c r="B28" s="50" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23">
+      <c r="B29" s="50" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23">
+      <c r="B30" s="50" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23">
+      <c r="B31" s="52" t="s">
+        <v>328</v>
+      </c>
+      <c r="C31" s="52"/>
+      <c r="D31" s="52"/>
+      <c r="E31" s="52"/>
+    </row>
+    <row r="32" spans="1:23">
+      <c r="B32" s="52" t="s">
+        <v>324</v>
+      </c>
+      <c r="C32" s="52"/>
+      <c r="D32" s="52"/>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="B33" s="52"/>
+      <c r="C33" s="52" t="s">
+        <v>325</v>
+      </c>
+      <c r="D33" s="52"/>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="B34" s="52"/>
+      <c r="C34" s="52" t="s">
+        <v>326</v>
+      </c>
+      <c r="D34" s="52"/>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="B35" s="52"/>
+      <c r="C35" s="52" t="s">
+        <v>327</v>
+      </c>
+      <c r="D35" s="52"/>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" s="54" t="s">
+        <v>339</v>
+      </c>
+      <c r="B37" s="50" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="B38" s="50" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="B39" s="53" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" s="69"/>
+      <c r="B40" s="53" t="s">
+        <v>342</v>
+      </c>
+      <c r="C40" s="53"/>
+      <c r="D40" s="53"/>
+      <c r="E40" s="53"/>
+      <c r="F40" s="53"/>
+      <c r="G40" s="53"/>
+      <c r="H40" s="53"/>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" s="69"/>
+      <c r="B41" s="53" t="s">
+        <v>344</v>
+      </c>
+      <c r="C41" s="53"/>
+      <c r="D41" s="53"/>
+      <c r="E41" s="53"/>
+      <c r="F41" s="53"/>
+      <c r="G41" s="53"/>
+      <c r="H41" s="53"/>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" s="69"/>
+      <c r="B42" s="53" t="s">
+        <v>345</v>
+      </c>
+      <c r="C42" s="53"/>
+      <c r="D42" s="53"/>
+      <c r="E42" s="53"/>
+      <c r="F42" s="53"/>
+      <c r="G42" s="53"/>
+      <c r="H42" s="53"/>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" s="69"/>
+      <c r="B43" s="53" t="s">
+        <v>346</v>
+      </c>
+      <c r="C43" s="53"/>
+      <c r="D43" s="53"/>
+      <c r="E43" s="53"/>
+      <c r="F43" s="53"/>
+      <c r="G43" s="53"/>
+      <c r="H43" s="53"/>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" s="69"/>
+      <c r="B44" s="53" t="s">
+        <v>346</v>
+      </c>
+      <c r="C44" s="53"/>
+      <c r="D44" s="53"/>
+      <c r="E44" s="53"/>
+      <c r="F44" s="53"/>
+      <c r="G44" s="53"/>
+      <c r="H44" s="53"/>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="B46" s="50" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="B47" s="50" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="B48" s="50" t="s">
+        <v>349</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3843DA9D-A47F-42DD-8648-F3AF22E69576}">
+  <dimension ref="B2:T36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col min="1" max="1" width="1.296875" customWidth="1"/>
+    <col min="2" max="2" width="2.8984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:20">
+      <c r="B2" s="50" t="s">
+        <v>287</v>
+      </c>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="52"/>
+      <c r="M2" s="52"/>
+      <c r="N2" s="52"/>
+      <c r="O2" s="52"/>
+      <c r="P2" s="52"/>
+      <c r="Q2" s="52"/>
+      <c r="R2" s="52"/>
+      <c r="S2" s="52"/>
+    </row>
+    <row r="3" spans="2:20">
+      <c r="B3" s="52" t="s">
+        <v>307</v>
+      </c>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="52"/>
+      <c r="L3" s="52"/>
+      <c r="M3" s="52"/>
+      <c r="N3" s="52"/>
+      <c r="O3" s="52"/>
+      <c r="P3" s="52"/>
+      <c r="Q3" s="52"/>
+      <c r="R3" s="52"/>
+      <c r="S3" s="52"/>
+    </row>
+    <row r="4" spans="2:20" ht="13.8" customHeight="1">
+      <c r="B4" s="52"/>
+      <c r="C4" s="62" t="s">
+        <v>313</v>
+      </c>
+      <c r="D4" s="62"/>
+      <c r="E4" s="62"/>
+      <c r="F4" s="62"/>
+      <c r="G4" s="62"/>
+      <c r="H4" s="62"/>
+      <c r="I4" s="62"/>
+      <c r="J4" s="62"/>
+      <c r="K4" s="62"/>
+      <c r="L4" s="62"/>
+      <c r="M4" s="62"/>
+      <c r="N4" s="62"/>
+      <c r="O4" s="62"/>
+      <c r="P4" s="62"/>
+      <c r="Q4" s="62"/>
+      <c r="R4" s="62"/>
+      <c r="S4" s="62"/>
+    </row>
+    <row r="5" spans="2:20">
+      <c r="B5" s="50"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
+      <c r="F5" s="62"/>
+      <c r="G5" s="62"/>
+      <c r="H5" s="62"/>
+      <c r="I5" s="62"/>
+      <c r="J5" s="62"/>
+      <c r="K5" s="62"/>
+      <c r="L5" s="62"/>
+      <c r="M5" s="62"/>
+      <c r="N5" s="62"/>
+      <c r="O5" s="62"/>
+      <c r="P5" s="62"/>
+      <c r="Q5" s="62"/>
+      <c r="R5" s="62"/>
+      <c r="S5" s="62"/>
+    </row>
+    <row r="6" spans="2:20">
+      <c r="B6" s="50"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="62"/>
+      <c r="F6" s="62"/>
+      <c r="G6" s="62"/>
+      <c r="H6" s="62"/>
+      <c r="I6" s="62"/>
+      <c r="J6" s="62"/>
+      <c r="K6" s="62"/>
+      <c r="L6" s="62"/>
+      <c r="M6" s="62"/>
+      <c r="N6" s="62"/>
+      <c r="O6" s="62"/>
+      <c r="P6" s="62"/>
+      <c r="Q6" s="62"/>
+      <c r="R6" s="62"/>
+      <c r="S6" s="62"/>
+    </row>
+    <row r="7" spans="2:20">
+      <c r="B7" s="50"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="50"/>
+      <c r="L7" s="50"/>
+      <c r="M7" s="50"/>
+      <c r="N7" s="50"/>
+      <c r="O7" s="50"/>
+      <c r="P7" s="50"/>
+      <c r="Q7" s="50"/>
+      <c r="R7" s="50"/>
+      <c r="S7" s="50"/>
+    </row>
+    <row r="8" spans="2:20">
+      <c r="B8" s="67" t="s">
+        <v>315</v>
+      </c>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="52"/>
+      <c r="G8" s="52"/>
+      <c r="H8" s="52"/>
+      <c r="I8" s="52"/>
+      <c r="J8" s="52"/>
+      <c r="K8" s="52"/>
+      <c r="L8" s="52"/>
+      <c r="M8" s="52"/>
+      <c r="N8" s="52"/>
+      <c r="O8" s="52"/>
+      <c r="P8" s="52"/>
+      <c r="Q8" s="52"/>
+      <c r="R8" s="52"/>
+      <c r="S8" s="50"/>
+      <c r="T8" s="1" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="9" spans="2:20">
+      <c r="B9" s="67" t="s">
+        <v>316</v>
+      </c>
+      <c r="C9" s="67"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="52"/>
+      <c r="F9" s="52"/>
+      <c r="G9" s="52"/>
+      <c r="H9" s="52"/>
+      <c r="I9" s="52"/>
+      <c r="J9" s="52"/>
+      <c r="K9" s="52"/>
+      <c r="L9" s="52"/>
+      <c r="M9" s="52"/>
+      <c r="N9" s="52"/>
+      <c r="O9" s="52"/>
+      <c r="P9" s="52"/>
+      <c r="Q9" s="52"/>
+      <c r="R9" s="52"/>
+      <c r="S9" s="50"/>
+    </row>
+    <row r="10" spans="2:20">
+      <c r="B10" s="67"/>
+      <c r="C10" s="67" t="s">
+        <v>317</v>
+      </c>
+      <c r="D10" s="52"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="52"/>
+      <c r="G10" s="52"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="52"/>
+      <c r="J10" s="52"/>
+      <c r="K10" s="52"/>
+      <c r="L10" s="52"/>
+      <c r="M10" s="52"/>
+      <c r="N10" s="52"/>
+      <c r="O10" s="52"/>
+      <c r="P10" s="52"/>
+      <c r="Q10" s="52"/>
+      <c r="R10" s="52"/>
+      <c r="S10" s="50"/>
+    </row>
+    <row r="12" spans="2:20">
+      <c r="B12" s="50" t="s">
+        <v>318</v>
+      </c>
+      <c r="C12" s="50"/>
+    </row>
+    <row r="14" spans="2:20">
+      <c r="B14" s="50" t="s">
+        <v>297</v>
+      </c>
+      <c r="C14" s="52"/>
+      <c r="D14" s="52"/>
+      <c r="E14" s="52"/>
+      <c r="F14" s="52"/>
+      <c r="G14" s="52"/>
+      <c r="H14" s="52"/>
+      <c r="I14" s="52"/>
+      <c r="J14" s="52"/>
+      <c r="K14" s="52"/>
+      <c r="L14" s="52"/>
+      <c r="M14" s="52"/>
+      <c r="N14" s="52"/>
+      <c r="O14" s="52"/>
+      <c r="P14" s="52"/>
+      <c r="Q14" s="52"/>
+    </row>
+    <row r="15" spans="2:20">
+      <c r="B15" s="52"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="52"/>
+      <c r="G15" s="52"/>
+      <c r="H15" s="52"/>
+      <c r="I15" s="52"/>
+      <c r="J15" s="52"/>
+      <c r="K15" s="52"/>
+      <c r="L15" s="52"/>
+      <c r="M15" s="52"/>
+      <c r="N15" s="52"/>
+      <c r="O15" s="52"/>
+      <c r="P15" s="52"/>
+      <c r="Q15" s="52"/>
+    </row>
+    <row r="16" spans="2:20">
+      <c r="B16" s="52" t="s">
+        <v>296</v>
+      </c>
+      <c r="C16" s="52"/>
+      <c r="D16" s="52"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="52"/>
+      <c r="G16" s="52"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="52"/>
+      <c r="J16" s="52"/>
+      <c r="K16" s="52"/>
+      <c r="L16" s="52"/>
+      <c r="M16" s="52"/>
+      <c r="N16" s="52"/>
+      <c r="O16" s="52"/>
+      <c r="P16" s="52"/>
+      <c r="Q16" s="52"/>
+    </row>
+    <row r="17" spans="2:17">
+      <c r="B17" s="52"/>
+      <c r="C17" s="52" t="s">
+        <v>290</v>
+      </c>
+      <c r="D17" s="52"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="52"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="52"/>
+      <c r="I17" s="52"/>
+      <c r="J17" s="52"/>
+      <c r="K17" s="52"/>
+      <c r="L17" s="52"/>
+      <c r="M17" s="52"/>
+      <c r="N17" s="52"/>
+      <c r="O17" s="52"/>
+      <c r="P17" s="52"/>
+      <c r="Q17" s="52"/>
+    </row>
+    <row r="18" spans="2:17">
+      <c r="B18" s="52"/>
+      <c r="C18" s="52" t="s">
+        <v>291</v>
+      </c>
+      <c r="D18" s="52"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="52"/>
+      <c r="G18" s="52"/>
+      <c r="H18" s="52"/>
+      <c r="I18" s="52"/>
+      <c r="J18" s="52"/>
+      <c r="K18" s="52"/>
+      <c r="L18" s="52"/>
+      <c r="M18" s="52"/>
+      <c r="N18" s="52"/>
+      <c r="O18" s="52"/>
+      <c r="P18" s="52"/>
+      <c r="Q18" s="52"/>
+    </row>
+    <row r="19" spans="2:17">
+      <c r="B19" s="52"/>
+      <c r="C19" s="52" t="s">
+        <v>292</v>
+      </c>
+      <c r="D19" s="52"/>
+      <c r="E19" s="52"/>
+      <c r="F19" s="52"/>
+      <c r="G19" s="52"/>
+      <c r="H19" s="52"/>
+      <c r="I19" s="52"/>
+      <c r="J19" s="52"/>
+      <c r="K19" s="52"/>
+      <c r="L19" s="52"/>
+      <c r="M19" s="52"/>
+      <c r="N19" s="52"/>
+      <c r="O19" s="52"/>
+      <c r="P19" s="52"/>
+      <c r="Q19" s="52"/>
+    </row>
+    <row r="20" spans="2:17">
+      <c r="B20" s="52"/>
+      <c r="C20" s="52" t="s">
+        <v>293</v>
+      </c>
+      <c r="D20" s="52"/>
+      <c r="E20" s="52"/>
+      <c r="F20" s="52"/>
+      <c r="G20" s="52"/>
+      <c r="H20" s="52"/>
+      <c r="I20" s="52"/>
+      <c r="J20" s="52"/>
+      <c r="K20" s="52"/>
+      <c r="L20" s="52"/>
+      <c r="M20" s="52"/>
+      <c r="N20" s="52"/>
+      <c r="O20" s="52"/>
+      <c r="P20" s="52"/>
+      <c r="Q20" s="52"/>
+    </row>
+    <row r="21" spans="2:17">
+      <c r="B21" s="52"/>
+      <c r="C21" s="52" t="s">
+        <v>294</v>
+      </c>
+      <c r="D21" s="52"/>
+      <c r="E21" s="52"/>
+      <c r="F21" s="52"/>
+      <c r="G21" s="52"/>
+      <c r="H21" s="52"/>
+      <c r="I21" s="52"/>
+      <c r="J21" s="52"/>
+      <c r="K21" s="52"/>
+      <c r="L21" s="52"/>
+      <c r="M21" s="52"/>
+      <c r="N21" s="52"/>
+      <c r="O21" s="52"/>
+      <c r="P21" s="52"/>
+      <c r="Q21" s="52"/>
+    </row>
+    <row r="22" spans="2:17">
       <c r="B22" s="52"/>
-      <c r="C22" s="52"/>
-      <c r="D22" s="52" t="s">
-        <v>294</v>
-      </c>
+      <c r="C22" s="52" t="s">
+        <v>295</v>
+      </c>
+      <c r="D22" s="52"/>
       <c r="E22" s="52"/>
       <c r="F22" s="52"/>
       <c r="G22" s="52"/>
@@ -8418,20 +9174,13 @@
       <c r="O22" s="52"/>
       <c r="P22" s="52"/>
       <c r="Q22" s="52"/>
-      <c r="R22" s="52"/>
-      <c r="S22" s="52"/>
-      <c r="T22" s="52"/>
-      <c r="U22" s="52"/>
-      <c r="V22" s="52"/>
-      <c r="W22" s="52"/>
-    </row>
-    <row r="23" spans="1:23">
-      <c r="A23" s="52"/>
+    </row>
+    <row r="23" spans="2:17">
       <c r="B23" s="52"/>
-      <c r="C23" s="52"/>
-      <c r="D23" s="52" t="s">
-        <v>295</v>
-      </c>
+      <c r="C23" s="52" t="s">
+        <v>298</v>
+      </c>
+      <c r="D23" s="52"/>
       <c r="E23" s="52"/>
       <c r="F23" s="52"/>
       <c r="G23" s="52"/>
@@ -8445,20 +9194,13 @@
       <c r="O23" s="52"/>
       <c r="P23" s="52"/>
       <c r="Q23" s="52"/>
-      <c r="R23" s="52"/>
-      <c r="S23" s="52"/>
-      <c r="T23" s="52"/>
-      <c r="U23" s="52"/>
-      <c r="V23" s="52"/>
-      <c r="W23" s="52"/>
-    </row>
-    <row r="24" spans="1:23">
-      <c r="A24" s="52"/>
+    </row>
+    <row r="24" spans="2:17">
       <c r="B24" s="52"/>
-      <c r="C24" s="52"/>
-      <c r="D24" s="52" t="s">
-        <v>296</v>
-      </c>
+      <c r="C24" s="52" t="s">
+        <v>299</v>
+      </c>
+      <c r="D24" s="52"/>
       <c r="E24" s="52"/>
       <c r="F24" s="52"/>
       <c r="G24" s="52"/>
@@ -8472,20 +9214,11 @@
       <c r="O24" s="52"/>
       <c r="P24" s="52"/>
       <c r="Q24" s="52"/>
-      <c r="R24" s="52"/>
-      <c r="S24" s="52"/>
-      <c r="T24" s="52"/>
-      <c r="U24" s="52"/>
-      <c r="V24" s="52"/>
-      <c r="W24" s="52"/>
-    </row>
-    <row r="25" spans="1:23">
-      <c r="A25" s="52"/>
+    </row>
+    <row r="25" spans="2:17">
       <c r="B25" s="52"/>
       <c r="C25" s="52"/>
-      <c r="D25" s="52" t="s">
-        <v>299</v>
-      </c>
+      <c r="D25" s="52"/>
       <c r="E25" s="52"/>
       <c r="F25" s="52"/>
       <c r="G25" s="52"/>
@@ -8499,20 +9232,13 @@
       <c r="O25" s="52"/>
       <c r="P25" s="52"/>
       <c r="Q25" s="52"/>
-      <c r="R25" s="52"/>
-      <c r="S25" s="52"/>
-      <c r="T25" s="52"/>
-      <c r="U25" s="52"/>
-      <c r="V25" s="52"/>
-      <c r="W25" s="52"/>
-    </row>
-    <row r="26" spans="1:23">
-      <c r="A26" s="52"/>
+    </row>
+    <row r="26" spans="2:17">
       <c r="B26" s="52"/>
-      <c r="C26" s="52"/>
-      <c r="D26" s="52" t="s">
-        <v>300</v>
-      </c>
+      <c r="C26" s="52" t="s">
+        <v>305</v>
+      </c>
+      <c r="D26" s="52"/>
       <c r="E26" s="52"/>
       <c r="F26" s="52"/>
       <c r="G26" s="52"/>
@@ -8526,17 +9252,12 @@
       <c r="O26" s="52"/>
       <c r="P26" s="52"/>
       <c r="Q26" s="52"/>
-      <c r="R26" s="52"/>
-      <c r="S26" s="52"/>
-      <c r="T26" s="52"/>
-      <c r="U26" s="52"/>
-      <c r="V26" s="52"/>
-      <c r="W26" s="52"/>
-    </row>
-    <row r="27" spans="1:23">
-      <c r="A27" s="52"/>
+    </row>
+    <row r="27" spans="2:17">
       <c r="B27" s="52"/>
-      <c r="C27" s="52"/>
+      <c r="C27" s="52" t="s">
+        <v>302</v>
+      </c>
       <c r="D27" s="52"/>
       <c r="E27" s="52"/>
       <c r="F27" s="52"/>
@@ -8551,20 +9272,13 @@
       <c r="O27" s="52"/>
       <c r="P27" s="52"/>
       <c r="Q27" s="52"/>
-      <c r="R27" s="52"/>
-      <c r="S27" s="52"/>
-      <c r="T27" s="52"/>
-      <c r="U27" s="52"/>
-      <c r="V27" s="52"/>
-      <c r="W27" s="52"/>
-    </row>
-    <row r="28" spans="1:23">
-      <c r="A28" s="52"/>
+    </row>
+    <row r="28" spans="2:17">
       <c r="B28" s="52"/>
-      <c r="C28" s="52"/>
-      <c r="D28" s="52" t="s">
-        <v>306</v>
-      </c>
+      <c r="C28" s="52" t="s">
+        <v>300</v>
+      </c>
+      <c r="D28" s="52"/>
       <c r="E28" s="52"/>
       <c r="F28" s="52"/>
       <c r="G28" s="52"/>
@@ -8578,20 +9292,13 @@
       <c r="O28" s="52"/>
       <c r="P28" s="52"/>
       <c r="Q28" s="52"/>
-      <c r="R28" s="52"/>
-      <c r="S28" s="52"/>
-      <c r="T28" s="52"/>
-      <c r="U28" s="52"/>
-      <c r="V28" s="52"/>
-      <c r="W28" s="52"/>
-    </row>
-    <row r="29" spans="1:23">
-      <c r="A29" s="52"/>
+    </row>
+    <row r="29" spans="2:17">
       <c r="B29" s="52"/>
-      <c r="C29" s="52"/>
-      <c r="D29" s="52" t="s">
-        <v>303</v>
-      </c>
+      <c r="C29" s="52" t="s">
+        <v>301</v>
+      </c>
+      <c r="D29" s="52"/>
       <c r="E29" s="52"/>
       <c r="F29" s="52"/>
       <c r="G29" s="52"/>
@@ -8605,20 +9312,13 @@
       <c r="O29" s="52"/>
       <c r="P29" s="52"/>
       <c r="Q29" s="52"/>
-      <c r="R29" s="52"/>
-      <c r="S29" s="52"/>
-      <c r="T29" s="52"/>
-      <c r="U29" s="52"/>
-      <c r="V29" s="52"/>
-      <c r="W29" s="52"/>
-    </row>
-    <row r="30" spans="1:23">
-      <c r="A30" s="52"/>
+    </row>
+    <row r="30" spans="2:17">
       <c r="B30" s="52"/>
-      <c r="C30" s="52"/>
-      <c r="D30" s="52" t="s">
-        <v>301</v>
-      </c>
+      <c r="C30" s="52" t="s">
+        <v>303</v>
+      </c>
+      <c r="D30" s="52"/>
       <c r="E30" s="52"/>
       <c r="F30" s="52"/>
       <c r="G30" s="52"/>
@@ -8632,20 +9332,13 @@
       <c r="O30" s="52"/>
       <c r="P30" s="52"/>
       <c r="Q30" s="52"/>
-      <c r="R30" s="52"/>
-      <c r="S30" s="52"/>
-      <c r="T30" s="52"/>
-      <c r="U30" s="52"/>
-      <c r="V30" s="52"/>
-      <c r="W30" s="52"/>
-    </row>
-    <row r="31" spans="1:23">
-      <c r="A31" s="52"/>
+    </row>
+    <row r="31" spans="2:17">
       <c r="B31" s="52"/>
-      <c r="C31" s="52"/>
-      <c r="D31" s="52" t="s">
-        <v>302</v>
-      </c>
+      <c r="C31" s="52" t="s">
+        <v>304</v>
+      </c>
+      <c r="D31" s="52"/>
       <c r="E31" s="52"/>
       <c r="F31" s="52"/>
       <c r="G31" s="52"/>
@@ -8659,606 +9352,57 @@
       <c r="O31" s="52"/>
       <c r="P31" s="52"/>
       <c r="Q31" s="52"/>
-      <c r="R31" s="52"/>
-      <c r="S31" s="52"/>
-      <c r="T31" s="52"/>
-      <c r="U31" s="52"/>
-      <c r="V31" s="52"/>
-      <c r="W31" s="52"/>
-    </row>
-    <row r="32" spans="1:23">
-      <c r="A32" s="52"/>
-      <c r="B32" s="52"/>
-      <c r="C32" s="52"/>
-      <c r="D32" s="52" t="s">
-        <v>304</v>
-      </c>
-      <c r="E32" s="52"/>
-      <c r="F32" s="52"/>
-      <c r="G32" s="52"/>
-      <c r="H32" s="52"/>
-      <c r="I32" s="52"/>
-      <c r="J32" s="52"/>
-      <c r="K32" s="52"/>
-      <c r="L32" s="52"/>
-      <c r="M32" s="52"/>
-      <c r="N32" s="52"/>
-      <c r="O32" s="52"/>
-      <c r="P32" s="52"/>
-      <c r="Q32" s="52"/>
-      <c r="R32" s="52"/>
-      <c r="S32" s="52"/>
-      <c r="T32" s="52"/>
-      <c r="U32" s="52"/>
-      <c r="V32" s="52"/>
-      <c r="W32" s="52"/>
-    </row>
-    <row r="33" spans="1:23">
-      <c r="A33" s="52"/>
-      <c r="B33" s="52"/>
-      <c r="C33" s="52"/>
-      <c r="D33" s="52" t="s">
-        <v>305</v>
-      </c>
-      <c r="E33" s="52"/>
-      <c r="F33" s="52"/>
-      <c r="G33" s="52"/>
-      <c r="H33" s="52"/>
-      <c r="I33" s="52"/>
-      <c r="J33" s="52"/>
-      <c r="K33" s="52"/>
-      <c r="L33" s="52"/>
-      <c r="M33" s="52"/>
-      <c r="N33" s="52"/>
-      <c r="O33" s="52"/>
-      <c r="P33" s="52"/>
-      <c r="Q33" s="52"/>
-      <c r="R33" s="52"/>
-      <c r="S33" s="52"/>
-      <c r="T33" s="52"/>
-      <c r="U33" s="52"/>
-      <c r="V33" s="52"/>
-      <c r="W33" s="52"/>
-    </row>
-    <row r="34" spans="1:23">
-      <c r="A34" s="52"/>
-      <c r="B34" s="52"/>
-      <c r="C34" s="52"/>
-      <c r="D34" s="52"/>
-      <c r="E34" s="52"/>
-      <c r="F34" s="52"/>
-      <c r="G34" s="52"/>
-      <c r="H34" s="52"/>
-      <c r="I34" s="52"/>
-      <c r="J34" s="52"/>
-      <c r="K34" s="52"/>
-      <c r="L34" s="52"/>
-      <c r="M34" s="52"/>
-      <c r="N34" s="52"/>
-      <c r="O34" s="52"/>
-      <c r="P34" s="52"/>
-      <c r="Q34" s="52"/>
-      <c r="R34" s="52"/>
-      <c r="S34" s="52"/>
-      <c r="T34" s="52"/>
-      <c r="U34" s="52"/>
-      <c r="V34" s="52"/>
-      <c r="W34" s="52"/>
-    </row>
-    <row r="35" spans="1:23">
-      <c r="A35" s="49" t="s">
-        <v>162</v>
-      </c>
-      <c r="B35" s="50" t="s">
-        <v>307</v>
-      </c>
-      <c r="F35" s="52"/>
-      <c r="G35" s="52"/>
-      <c r="H35" s="52"/>
-      <c r="I35" s="52"/>
-      <c r="J35" s="52"/>
-      <c r="K35" s="52"/>
-      <c r="L35" s="52"/>
-      <c r="M35" s="52"/>
-      <c r="N35" s="52"/>
-      <c r="O35" s="52"/>
-      <c r="P35" s="52"/>
-      <c r="Q35" s="52"/>
-      <c r="R35" s="52"/>
-      <c r="S35" s="52"/>
-      <c r="T35" s="52"/>
-      <c r="U35" s="52"/>
-      <c r="V35" s="52"/>
-      <c r="W35" s="52"/>
-    </row>
-    <row r="36" spans="1:23">
-      <c r="A36" s="52"/>
+    </row>
+    <row r="33" spans="3:8">
+      <c r="C33" s="52" t="s">
+        <v>311</v>
+      </c>
+      <c r="D33" s="50"/>
+      <c r="E33" s="50"/>
+      <c r="F33" s="50"/>
+      <c r="G33" s="50"/>
+      <c r="H33" s="50"/>
+    </row>
+    <row r="34" spans="3:8">
+      <c r="C34" s="52" t="s">
+        <v>308</v>
+      </c>
+      <c r="D34" s="50"/>
+      <c r="E34" s="50"/>
+      <c r="F34" s="50"/>
+      <c r="G34" s="50"/>
+      <c r="H34" s="50"/>
+    </row>
+    <row r="35" spans="3:8">
+      <c r="C35" s="52" t="s">
+        <v>309</v>
+      </c>
+      <c r="D35" s="50"/>
+      <c r="E35" s="50"/>
+      <c r="F35" s="50"/>
+      <c r="G35" s="50"/>
+      <c r="H35" s="50"/>
+    </row>
+    <row r="36" spans="3:8">
       <c r="C36" s="52" t="s">
-        <v>315</v>
-      </c>
-      <c r="F36" s="52"/>
-      <c r="G36" s="52"/>
-      <c r="H36" s="52"/>
-      <c r="I36" s="52"/>
-      <c r="J36" s="52"/>
-      <c r="K36" s="52"/>
-      <c r="L36" s="52"/>
-      <c r="M36" s="52"/>
-      <c r="N36" s="52"/>
-      <c r="O36" s="52"/>
-      <c r="P36" s="52"/>
-      <c r="Q36" s="52"/>
-      <c r="R36" s="52"/>
-      <c r="S36" s="52"/>
-      <c r="T36" s="52"/>
-      <c r="U36" s="52"/>
-      <c r="V36" s="52"/>
-      <c r="W36" s="52"/>
-    </row>
-    <row r="37" spans="1:23">
-      <c r="A37" s="52"/>
-      <c r="C37" s="52" t="s">
-        <v>313</v>
-      </c>
-      <c r="F37" s="52"/>
-      <c r="G37" s="52"/>
-      <c r="H37" s="52"/>
-      <c r="I37" s="52"/>
-      <c r="J37" s="52"/>
-      <c r="K37" s="52"/>
-      <c r="L37" s="52"/>
-      <c r="M37" s="52"/>
-      <c r="N37" s="52"/>
-      <c r="O37" s="52"/>
-      <c r="P37" s="52"/>
-      <c r="Q37" s="52"/>
-      <c r="R37" s="52"/>
-      <c r="S37" s="52"/>
-      <c r="T37" s="52"/>
-      <c r="U37" s="52"/>
-      <c r="V37" s="52"/>
-      <c r="W37" s="52"/>
-    </row>
-    <row r="38" spans="1:23">
-      <c r="A38" s="52"/>
-      <c r="B38" s="52"/>
-      <c r="C38" s="50" t="s">
-        <v>288</v>
-      </c>
-      <c r="D38" s="52"/>
-      <c r="E38" s="52"/>
-      <c r="F38" s="52"/>
-      <c r="G38" s="52"/>
-      <c r="H38" s="52"/>
-      <c r="I38" s="52"/>
-      <c r="J38" s="52"/>
-      <c r="K38" s="52"/>
-      <c r="L38" s="52"/>
-      <c r="M38" s="52"/>
-      <c r="N38" s="52"/>
-      <c r="O38" s="52"/>
-      <c r="P38" s="52"/>
-      <c r="Q38" s="52"/>
-      <c r="R38" s="52"/>
-      <c r="S38" s="52"/>
-      <c r="T38" s="52"/>
-      <c r="U38" s="52"/>
-      <c r="V38" s="52"/>
-      <c r="W38" s="52"/>
-    </row>
-    <row r="39" spans="1:23">
-      <c r="A39" s="50"/>
-      <c r="B39" s="52"/>
-      <c r="C39" s="52" t="s">
-        <v>308</v>
-      </c>
-      <c r="D39" s="52"/>
-      <c r="E39" s="52"/>
-      <c r="F39" s="52"/>
-      <c r="G39" s="52"/>
-      <c r="H39" s="52"/>
-      <c r="I39" s="52"/>
-      <c r="J39" s="52"/>
-      <c r="K39" s="52"/>
-      <c r="L39" s="52"/>
-      <c r="M39" s="52"/>
-      <c r="N39" s="52"/>
-      <c r="O39" s="52"/>
-      <c r="P39" s="52"/>
-      <c r="Q39" s="52"/>
-      <c r="R39" s="52"/>
-      <c r="S39" s="52"/>
-      <c r="T39" s="52"/>
-      <c r="U39" s="52"/>
-      <c r="V39" s="52"/>
-      <c r="W39" s="52"/>
-    </row>
-    <row r="40" spans="1:23">
-      <c r="C40" s="52"/>
-      <c r="D40" s="66" t="s">
-        <v>314</v>
-      </c>
-      <c r="E40" s="66"/>
-      <c r="F40" s="66"/>
-      <c r="G40" s="66"/>
-      <c r="H40" s="66"/>
-      <c r="I40" s="66"/>
-      <c r="J40" s="66"/>
-      <c r="K40" s="66"/>
-      <c r="L40" s="66"/>
-      <c r="M40" s="66"/>
-      <c r="N40" s="66"/>
-      <c r="O40" s="66"/>
-      <c r="P40" s="66"/>
-      <c r="Q40" s="66"/>
-      <c r="R40" s="66"/>
-      <c r="S40" s="66"/>
-      <c r="T40" s="66"/>
-    </row>
-    <row r="41" spans="1:23">
-      <c r="D41" s="66"/>
-      <c r="E41" s="66"/>
-      <c r="F41" s="66"/>
-      <c r="G41" s="66"/>
-      <c r="H41" s="66"/>
-      <c r="I41" s="66"/>
-      <c r="J41" s="66"/>
-      <c r="K41" s="66"/>
-      <c r="L41" s="66"/>
-      <c r="M41" s="66"/>
-      <c r="N41" s="66"/>
-      <c r="O41" s="66"/>
-      <c r="P41" s="66"/>
-      <c r="Q41" s="66"/>
-      <c r="R41" s="66"/>
-      <c r="S41" s="66"/>
-      <c r="T41" s="66"/>
-    </row>
-    <row r="42" spans="1:23">
-      <c r="D42" s="66"/>
-      <c r="E42" s="66"/>
-      <c r="F42" s="66"/>
-      <c r="G42" s="66"/>
-      <c r="H42" s="66"/>
-      <c r="I42" s="66"/>
-      <c r="J42" s="66"/>
-      <c r="K42" s="66"/>
-      <c r="L42" s="66"/>
-      <c r="M42" s="66"/>
-      <c r="N42" s="66"/>
-      <c r="O42" s="66"/>
-      <c r="P42" s="66"/>
-      <c r="Q42" s="66"/>
-      <c r="R42" s="66"/>
-      <c r="S42" s="66"/>
-      <c r="T42" s="66"/>
-    </row>
-    <row r="43" spans="1:23">
-      <c r="C43" s="50" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="44" spans="1:23">
-      <c r="C44" s="52" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="45" spans="1:23">
-      <c r="C45" s="52" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="46" spans="1:23">
-      <c r="C46" s="52" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="47" spans="1:23">
-      <c r="C47" s="52" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="48" spans="1:23">
-      <c r="B48" s="52"/>
-      <c r="C48" s="52"/>
-      <c r="D48" s="52"/>
-      <c r="E48" s="52"/>
-      <c r="F48" s="52"/>
-      <c r="G48" s="52"/>
-      <c r="H48" s="52"/>
-      <c r="I48" s="52"/>
-      <c r="J48" s="52"/>
-      <c r="K48" s="52"/>
-      <c r="L48" s="52"/>
-      <c r="M48" s="52"/>
-      <c r="N48" s="52"/>
-      <c r="O48" s="52"/>
-      <c r="P48" s="52"/>
-      <c r="Q48" s="52"/>
-      <c r="R48" s="52"/>
-      <c r="S48" s="52"/>
-    </row>
-    <row r="49" spans="1:19">
-      <c r="B49" s="52"/>
-      <c r="C49" s="52" t="s">
-        <v>316</v>
-      </c>
-      <c r="D49" s="52"/>
-      <c r="E49" s="52"/>
-      <c r="F49" s="52"/>
-      <c r="G49" s="52"/>
-      <c r="H49" s="52"/>
-      <c r="I49" s="52"/>
-      <c r="J49" s="52"/>
-      <c r="K49" s="52"/>
-      <c r="L49" s="52"/>
-      <c r="M49" s="52"/>
-      <c r="N49" s="52"/>
-      <c r="O49" s="52"/>
-      <c r="P49" s="52"/>
-      <c r="Q49" s="52"/>
-      <c r="R49" s="52"/>
-      <c r="S49" s="52"/>
-    </row>
-    <row r="50" spans="1:19">
-      <c r="B50" s="52"/>
-      <c r="C50" s="50" t="s">
-        <v>288</v>
-      </c>
-      <c r="D50" s="52"/>
-      <c r="E50" s="52"/>
-      <c r="F50" s="52"/>
-      <c r="G50" s="52"/>
-      <c r="H50" s="52"/>
-      <c r="I50" s="52"/>
-      <c r="J50" s="52"/>
-      <c r="K50" s="52"/>
-      <c r="L50" s="52"/>
-      <c r="M50" s="52"/>
-      <c r="N50" s="52"/>
-      <c r="O50" s="52"/>
-      <c r="P50" s="52"/>
-      <c r="Q50" s="52"/>
-      <c r="R50" s="52"/>
-      <c r="S50" s="52"/>
-    </row>
-    <row r="51" spans="1:19">
-      <c r="B51" s="52"/>
-      <c r="C51" s="52" t="s">
-        <v>317</v>
-      </c>
-      <c r="D51" s="52"/>
-      <c r="E51" s="52"/>
-      <c r="F51" s="52"/>
-      <c r="G51" s="52"/>
-      <c r="H51" s="52"/>
-      <c r="I51" s="52"/>
-      <c r="J51" s="52"/>
-      <c r="K51" s="52"/>
-      <c r="L51" s="52"/>
-      <c r="M51" s="52"/>
-      <c r="N51" s="52"/>
-      <c r="O51" s="52"/>
-      <c r="P51" s="52"/>
-      <c r="Q51" s="52"/>
-      <c r="R51" s="52"/>
-      <c r="S51" s="52"/>
-    </row>
-    <row r="52" spans="1:19">
-      <c r="B52" s="52"/>
-      <c r="C52" s="52"/>
-      <c r="D52" s="52" t="s">
-        <v>318</v>
-      </c>
-      <c r="E52" s="52"/>
-      <c r="F52" s="52"/>
-      <c r="G52" s="52"/>
-      <c r="H52" s="52"/>
-      <c r="I52" s="52"/>
-      <c r="J52" s="52"/>
-      <c r="K52" s="52"/>
-      <c r="L52" s="52"/>
-      <c r="M52" s="52"/>
-      <c r="N52" s="52"/>
-      <c r="O52" s="52"/>
-      <c r="P52" s="52"/>
-      <c r="Q52" s="52"/>
-      <c r="R52" s="52"/>
-      <c r="S52" s="52"/>
-    </row>
-    <row r="53" spans="1:19">
-      <c r="B53" s="52"/>
-      <c r="C53" s="52"/>
-      <c r="D53" s="52"/>
-      <c r="E53" s="52"/>
-      <c r="F53" s="52"/>
-      <c r="G53" s="52"/>
-      <c r="H53" s="52"/>
-      <c r="I53" s="52"/>
-      <c r="J53" s="52"/>
-      <c r="K53" s="52"/>
-      <c r="L53" s="52"/>
-      <c r="M53" s="52"/>
-      <c r="N53" s="52"/>
-      <c r="O53" s="52"/>
-      <c r="P53" s="52"/>
-      <c r="Q53" s="52"/>
-      <c r="R53" s="52"/>
-      <c r="S53" s="52"/>
-    </row>
-    <row r="54" spans="1:19">
-      <c r="B54" s="52"/>
-      <c r="C54" s="52"/>
-      <c r="D54" s="52"/>
-      <c r="E54" s="52"/>
-      <c r="F54" s="52"/>
-      <c r="G54" s="52"/>
-      <c r="H54" s="52"/>
-      <c r="I54" s="52"/>
-      <c r="J54" s="52"/>
-      <c r="K54" s="52"/>
-      <c r="L54" s="52"/>
-      <c r="M54" s="52"/>
-      <c r="N54" s="52"/>
-      <c r="O54" s="52"/>
-      <c r="P54" s="52"/>
-      <c r="Q54" s="52"/>
-      <c r="R54" s="52"/>
-      <c r="S54" s="52"/>
-    </row>
-    <row r="55" spans="1:19">
-      <c r="A55" s="49" t="s">
-        <v>162</v>
-      </c>
-      <c r="B55" s="50" t="s">
-        <v>319</v>
-      </c>
-      <c r="E55" s="52"/>
-      <c r="F55" s="52"/>
-      <c r="G55" s="52"/>
-      <c r="H55" s="52"/>
-      <c r="I55" s="52"/>
-      <c r="J55" s="52"/>
-      <c r="K55" s="52"/>
-      <c r="L55" s="52"/>
-      <c r="M55" s="52"/>
-      <c r="N55" s="52"/>
-      <c r="O55" s="52"/>
-      <c r="P55" s="52"/>
-      <c r="Q55" s="52"/>
-      <c r="R55" s="52"/>
-      <c r="S55" s="52"/>
-    </row>
-    <row r="56" spans="1:19">
-      <c r="B56" s="52"/>
-      <c r="C56" s="52"/>
-      <c r="D56" s="52"/>
-      <c r="E56" s="52"/>
-      <c r="F56" s="52"/>
-      <c r="G56" s="52"/>
-      <c r="H56" s="52"/>
-      <c r="I56" s="52"/>
-      <c r="J56" s="52"/>
-      <c r="K56" s="52"/>
-      <c r="L56" s="52"/>
-      <c r="M56" s="52"/>
-      <c r="N56" s="52"/>
-      <c r="O56" s="52"/>
-      <c r="P56" s="52"/>
-      <c r="Q56" s="52"/>
-      <c r="R56" s="52"/>
-      <c r="S56" s="52"/>
-    </row>
-    <row r="57" spans="1:19">
-      <c r="B57" s="52"/>
-      <c r="C57" s="52"/>
-      <c r="D57" s="52"/>
-      <c r="E57" s="52"/>
-      <c r="F57" s="52"/>
-      <c r="G57" s="52"/>
-      <c r="H57" s="52"/>
-      <c r="I57" s="52"/>
-      <c r="J57" s="52"/>
-      <c r="K57" s="52"/>
-      <c r="L57" s="52"/>
-      <c r="M57" s="52"/>
-      <c r="N57" s="52"/>
-      <c r="O57" s="52"/>
-      <c r="P57" s="52"/>
-      <c r="Q57" s="52"/>
-      <c r="R57" s="52"/>
-      <c r="S57" s="52"/>
-    </row>
-    <row r="58" spans="1:19">
-      <c r="B58" s="52"/>
-      <c r="C58" s="52"/>
-      <c r="D58" s="52"/>
-      <c r="E58" s="52"/>
-      <c r="F58" s="52"/>
-      <c r="G58" s="52"/>
-      <c r="H58" s="52"/>
-      <c r="I58" s="52"/>
-      <c r="J58" s="52"/>
-      <c r="K58" s="52"/>
-      <c r="L58" s="52"/>
-      <c r="M58" s="52"/>
-      <c r="N58" s="52"/>
-      <c r="O58" s="52"/>
-      <c r="P58" s="52"/>
-      <c r="Q58" s="52"/>
-      <c r="R58" s="52"/>
-      <c r="S58" s="52"/>
-    </row>
-    <row r="59" spans="1:19">
-      <c r="B59" s="52"/>
-      <c r="C59" s="52"/>
-      <c r="D59" s="52"/>
-      <c r="E59" s="52"/>
-      <c r="F59" s="52"/>
-      <c r="G59" s="52"/>
-      <c r="H59" s="52"/>
-      <c r="I59" s="52"/>
-      <c r="J59" s="52"/>
-      <c r="K59" s="52"/>
-      <c r="L59" s="52"/>
-      <c r="M59" s="52"/>
-      <c r="N59" s="52"/>
-      <c r="O59" s="52"/>
-      <c r="P59" s="52"/>
-      <c r="Q59" s="52"/>
-      <c r="R59" s="52"/>
-      <c r="S59" s="52"/>
-    </row>
-    <row r="60" spans="1:19">
-      <c r="B60" s="52"/>
-      <c r="C60" s="52"/>
-      <c r="D60" s="52"/>
-      <c r="E60" s="52"/>
-      <c r="F60" s="52"/>
-      <c r="G60" s="52"/>
-      <c r="H60" s="52"/>
-      <c r="I60" s="52"/>
-      <c r="J60" s="52"/>
-      <c r="K60" s="52"/>
-      <c r="L60" s="52"/>
-      <c r="M60" s="52"/>
-      <c r="N60" s="52"/>
-      <c r="O60" s="52"/>
-      <c r="P60" s="52"/>
-      <c r="Q60" s="52"/>
-      <c r="R60" s="52"/>
-      <c r="S60" s="52"/>
-    </row>
-    <row r="61" spans="1:19">
-      <c r="B61" s="52"/>
-      <c r="C61" s="52"/>
-      <c r="D61" s="52"/>
-      <c r="E61" s="52"/>
-      <c r="F61" s="52"/>
-      <c r="G61" s="52"/>
-      <c r="H61" s="52"/>
-      <c r="I61" s="52"/>
-      <c r="J61" s="52"/>
-      <c r="K61" s="52"/>
-      <c r="L61" s="52"/>
-      <c r="M61" s="52"/>
-      <c r="N61" s="52"/>
-      <c r="O61" s="52"/>
-      <c r="P61" s="52"/>
-      <c r="Q61" s="52"/>
-      <c r="R61" s="52"/>
-      <c r="S61" s="52"/>
+      <c r="D36" s="50"/>
+      <c r="E36" s="50"/>
+      <c r="F36" s="50"/>
+      <c r="G36" s="50"/>
+      <c r="H36" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D40:T42"/>
+    <mergeCell ref="C4:S6"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5662CF2F-C597-4142-B5A6-A1A36896CB7A}">
   <dimension ref="B2:T32"/>
   <sheetViews>
@@ -9316,18 +9460,18 @@
     </row>
     <row r="6" spans="2:20" ht="4.8" customHeight="1">
       <c r="B6" s="25"/>
-      <c r="C6" s="63" t="s">
+      <c r="C6" s="64" t="s">
         <v>112</v>
       </c>
-      <c r="D6" s="63"/>
-      <c r="E6" s="63"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="64"/>
       <c r="F6" s="26"/>
       <c r="H6" s="25"/>
-      <c r="I6" s="63" t="s">
+      <c r="I6" s="64" t="s">
         <v>113</v>
       </c>
-      <c r="J6" s="63"/>
-      <c r="K6" s="63"/>
+      <c r="J6" s="64"/>
+      <c r="K6" s="64"/>
       <c r="L6" s="42"/>
       <c r="M6" s="26"/>
       <c r="N6" s="27"/>
@@ -9502,11 +9646,11 @@
     </row>
     <row r="15" spans="2:20" ht="22.2" customHeight="1">
       <c r="B15" s="25"/>
-      <c r="C15" s="62" t="s">
+      <c r="C15" s="63" t="s">
         <v>111</v>
       </c>
-      <c r="D15" s="62"/>
-      <c r="E15" s="62"/>
+      <c r="D15" s="63"/>
+      <c r="E15" s="63"/>
       <c r="F15" s="26"/>
       <c r="H15" s="25"/>
       <c r="I15" s="30" t="s">
@@ -9579,11 +9723,11 @@
     </row>
     <row r="21" spans="2:16" ht="4.8" customHeight="1">
       <c r="B21" s="25"/>
-      <c r="C21" s="63" t="s">
+      <c r="C21" s="64" t="s">
         <v>133</v>
       </c>
-      <c r="D21" s="63"/>
-      <c r="E21" s="63"/>
+      <c r="D21" s="64"/>
+      <c r="E21" s="64"/>
       <c r="F21" s="26"/>
     </row>
     <row r="22" spans="2:16" ht="22.2" customHeight="1">
@@ -9727,11 +9871,11 @@
     </row>
     <row r="31" spans="2:16" ht="22.2" customHeight="1">
       <c r="B31" s="25"/>
-      <c r="C31" s="62" t="s">
+      <c r="C31" s="63" t="s">
         <v>111</v>
       </c>
-      <c r="D31" s="62"/>
-      <c r="E31" s="62"/>
+      <c r="D31" s="63"/>
+      <c r="E31" s="63"/>
       <c r="F31" s="26"/>
       <c r="H31" s="44"/>
       <c r="I31" s="44"/>
@@ -9758,12 +9902,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE199072-3796-4822-8475-BE7830E0C19A}">
   <dimension ref="A2:Z74"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="Z3" sqref="Z3"/>
+    <sheetView showGridLines="0" topLeftCell="A12" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AG40" sqref="AG40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -9784,7 +9928,7 @@
         <v>163</v>
       </c>
       <c r="Z3" t="s">
-        <v>166</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:26">
@@ -9827,14 +9971,14 @@
         <v>164</v>
       </c>
       <c r="Z26" t="s">
-        <v>165</v>
+        <v>319</v>
       </c>
     </row>
     <row r="27" spans="9:26">
       <c r="I27" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="Z27" t="s">
+      <c r="Z27" s="4" t="s">
         <v>165</v>
       </c>
     </row>
@@ -9845,6 +9989,9 @@
       <c r="J28" t="s">
         <v>96</v>
       </c>
+      <c r="Z28" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="29" spans="9:26">
       <c r="I29" t="s">
@@ -9853,17 +10000,20 @@
       <c r="J29" t="s">
         <v>83</v>
       </c>
+      <c r="Z29" t="s">
+        <v>320</v>
+      </c>
     </row>
     <row r="30" spans="9:26" ht="14.4" thickBot="1"/>
     <row r="31" spans="9:26">
-      <c r="I31" s="64" t="s">
+      <c r="I31" s="65" t="s">
         <v>89</v>
       </c>
-      <c r="J31" s="65"/>
-      <c r="K31" s="65"/>
-      <c r="L31" s="65"/>
-      <c r="M31" s="65"/>
-      <c r="N31" s="65"/>
+      <c r="J31" s="66"/>
+      <c r="K31" s="66"/>
+      <c r="L31" s="66"/>
+      <c r="M31" s="66"/>
+      <c r="N31" s="66"/>
       <c r="O31" s="12"/>
       <c r="P31" s="12"/>
       <c r="Q31" s="12"/>
@@ -9981,16 +10131,19 @@
   <mergeCells count="1">
     <mergeCell ref="I31:N31"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="Z27" r:id="rId1" xr:uid="{B918E269-1BC5-46C5-8127-2D6CB8595C41}"/>
+  </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;1#&amp;"Trebuchet MS"&amp;9&amp;K737373PÚBLICA</oddFooter>
   </headerFooter>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF806374-C006-4CAA-A186-B52BAD2C3D52}">
   <dimension ref="A1:A157"/>
   <sheetViews>
@@ -10005,32 +10158,32 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="56" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="56" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="56" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="56" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="56" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="56" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="13.8">
@@ -10038,17 +10191,17 @@
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="58" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="59" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="59" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="13.8">
@@ -10056,32 +10209,32 @@
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="58" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="59" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="59" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="59" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="59" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="59" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="13.8">
@@ -10092,32 +10245,32 @@
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="58" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" s="56" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="56" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="56" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="56" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" s="56" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="13.8">
@@ -10125,17 +10278,17 @@
     </row>
     <row r="27" spans="1:1">
       <c r="A27" s="58" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" s="60" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" s="60" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="13.8">
@@ -10143,12 +10296,12 @@
     </row>
     <row r="31" spans="1:1">
       <c r="A31" s="58" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" s="60" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="13.8">
@@ -10156,17 +10309,17 @@
     </row>
     <row r="34" spans="1:1">
       <c r="A34" s="60" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" s="60" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" s="60" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="37" spans="1:1" ht="13.8">
@@ -10174,7 +10327,7 @@
     </row>
     <row r="38" spans="1:1">
       <c r="A38" s="60" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="39" spans="1:1" ht="13.8">
@@ -10182,7 +10335,7 @@
     </row>
     <row r="40" spans="1:1">
       <c r="A40" s="59" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="41" spans="1:1" ht="13.8">
@@ -10190,12 +10343,12 @@
     </row>
     <row r="42" spans="1:1">
       <c r="A42" s="60" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" s="60" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="44" spans="1:1" ht="13.8">
@@ -10203,22 +10356,22 @@
     </row>
     <row r="45" spans="1:1">
       <c r="A45" s="60" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" s="60" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" s="60" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" s="60" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="49" spans="1:1" ht="13.8">
@@ -10226,12 +10379,12 @@
     </row>
     <row r="50" spans="1:1">
       <c r="A50" s="60" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" s="60" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="52" spans="1:1" ht="13.8">
@@ -10239,52 +10392,52 @@
     </row>
     <row r="53" spans="1:1">
       <c r="A53" s="58" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" s="60" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" s="60" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" s="60" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" s="58" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" s="60" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" s="60" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60" s="60" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" s="60" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" s="60" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="63" spans="1:1" ht="13.8">
@@ -10292,12 +10445,12 @@
     </row>
     <row r="64" spans="1:1">
       <c r="A64" s="60" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" s="60" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="66" spans="1:1">
@@ -10310,37 +10463,37 @@
     </row>
     <row r="68" spans="1:1">
       <c r="A68" s="58" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" s="59" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" s="60" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" s="60" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" s="60" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73" s="60" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74" s="60" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="75" spans="1:1" ht="13.8">
@@ -10348,17 +10501,17 @@
     </row>
     <row r="76" spans="1:1">
       <c r="A76" s="60" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77" s="60" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" s="60" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="79" spans="1:1">
@@ -10368,7 +10521,7 @@
     </row>
     <row r="80" spans="1:1">
       <c r="A80" s="58" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="81" spans="1:1" ht="13.8">
@@ -10376,12 +10529,12 @@
     </row>
     <row r="82" spans="1:1">
       <c r="A82" s="58" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83" s="59" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="84" spans="1:1" ht="13.8">
@@ -10389,37 +10542,37 @@
     </row>
     <row r="85" spans="1:1">
       <c r="A85" s="58" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="86" spans="1:1">
       <c r="A86" s="60" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="87" spans="1:1">
       <c r="A87" s="60" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88" s="60" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="89" spans="1:1">
       <c r="A89" s="60" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="90" spans="1:1">
       <c r="A90" s="60" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="91" spans="1:1">
       <c r="A91" s="60" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="92" spans="1:1" ht="13.8">
@@ -10427,42 +10580,42 @@
     </row>
     <row r="93" spans="1:1">
       <c r="A93" s="58" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="94" spans="1:1">
       <c r="A94" s="58" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="95" spans="1:1">
       <c r="A95" s="60" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="96" spans="1:1">
       <c r="A96" s="60" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="97" spans="1:1">
       <c r="A97" s="58" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="98" spans="1:1">
       <c r="A98" s="60" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99" s="60" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="100" spans="1:1">
       <c r="A100" s="60" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="101" spans="1:1" ht="13.8">
@@ -10470,27 +10623,27 @@
     </row>
     <row r="102" spans="1:1">
       <c r="A102" s="58" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103" s="60" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="104" spans="1:1">
       <c r="A104" s="60" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="105" spans="1:1">
       <c r="A105" s="60" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="106" spans="1:1">
       <c r="A106" s="60" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="107" spans="1:1" ht="13.8">
@@ -10498,17 +10651,17 @@
     </row>
     <row r="108" spans="1:1">
       <c r="A108" s="58" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="109" spans="1:1">
       <c r="A109" s="60" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="110" spans="1:1">
       <c r="A110" s="60" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="111" spans="1:1" ht="13.8">
@@ -10516,32 +10669,32 @@
     </row>
     <row r="112" spans="1:1">
       <c r="A112" s="60" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="113" spans="1:1">
       <c r="A113" s="60" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="114" spans="1:1">
       <c r="A114" s="60" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="115" spans="1:1">
       <c r="A115" s="60" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="116" spans="1:1">
       <c r="A116" s="60" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="117" spans="1:1">
       <c r="A117" s="60" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="118" spans="1:1" ht="13.8">
@@ -10549,27 +10702,27 @@
     </row>
     <row r="119" spans="1:1">
       <c r="A119" s="58" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="120" spans="1:1">
       <c r="A120" s="58" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="121" spans="1:1">
       <c r="A121" s="59" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="122" spans="1:1">
       <c r="A122" s="60" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="123" spans="1:1">
       <c r="A123" s="60" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="124" spans="1:1" ht="13.8">
@@ -10577,12 +10730,12 @@
     </row>
     <row r="125" spans="1:1">
       <c r="A125" s="60" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="126" spans="1:1">
       <c r="A126" s="60" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="127" spans="1:1" ht="13.8">
@@ -10590,57 +10743,57 @@
     </row>
     <row r="128" spans="1:1">
       <c r="A128" s="58" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="129" spans="1:1">
       <c r="A129" s="60" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="130" spans="1:1">
       <c r="A130" s="60" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="131" spans="1:1">
       <c r="A131" s="60" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="132" spans="1:1">
       <c r="A132" s="60" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="133" spans="1:1">
       <c r="A133" s="60" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="134" spans="1:1">
       <c r="A134" s="60" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="135" spans="1:1">
       <c r="A135" s="60" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="136" spans="1:1">
       <c r="A136" s="60" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="137" spans="1:1">
       <c r="A137" s="60" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="138" spans="1:1">
       <c r="A138" s="60" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="139" spans="1:1" ht="13.8">
@@ -10648,77 +10801,77 @@
     </row>
     <row r="140" spans="1:1">
       <c r="A140" s="58" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="141" spans="1:1">
       <c r="A141" s="60" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="142" spans="1:1">
       <c r="A142" s="60" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="143" spans="1:1">
       <c r="A143" s="60" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="144" spans="1:1">
       <c r="A144" s="60" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="145" spans="1:1">
       <c r="A145" s="60" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="146" spans="1:1">
       <c r="A146" s="60" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="147" spans="1:1">
       <c r="A147" s="60" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="148" spans="1:1">
       <c r="A148" s="60" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="149" spans="1:1">
       <c r="A149" s="60" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="150" spans="1:1">
       <c r="A150" s="60" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="151" spans="1:1">
       <c r="A151" s="60" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="152" spans="1:1">
       <c r="A152" s="60" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="153" spans="1:1">
       <c r="A153" s="60" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="154" spans="1:1">
       <c r="A154" s="60" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="155" spans="1:1" ht="13.8">
@@ -10726,7 +10879,7 @@
     </row>
     <row r="156" spans="1:1">
       <c r="A156" s="60" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="157" spans="1:1">
@@ -10739,7 +10892,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B1EFC28-03AD-49B3-A34B-C774469066CB}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -10768,7 +10921,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DD457A7-FD2E-4C2D-95B2-ABAD37EB7802}">
   <dimension ref="A1:Q90"/>
   <sheetViews>

</xml_diff>